<commit_message>
some boring codes completed
</commit_message>
<xml_diff>
--- a/数据库设计.xlsx
+++ b/数据库设计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="157">
   <si>
     <t>学号（id）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -637,6 +637,14 @@
   </si>
   <si>
     <t>要不要绩点学分呢?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tname</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -962,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1600,254 +1608,254 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>1</v>
-      </c>
-      <c r="G43" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>95</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>133</v>
-      </c>
-      <c r="B47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" t="s">
-        <v>14</v>
+      <c r="D46">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="F49">
+      <c r="E49">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
       <c r="G50" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D51">
         <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>136</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>137</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>138</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" t="s">
-        <v>14</v>
+      <c r="D53">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="F57">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>109</v>
+      <c r="F58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D59">
         <v>1</v>
+      </c>
+      <c r="G59" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1855,10 +1863,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" t="s">
         <v>103</v>
@@ -1867,8 +1875,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>